<commit_message>
Search students, teachers and courses
</commit_message>
<xml_diff>
--- a/Docs/BugImprovTracking.xlsx
+++ b/Docs/BugImprovTracking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t xml:space="preserve">Bug Tracking</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Insert option to add more than 2 parents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clear button to clear data for new search / take off delete</t>
   </si>
 </sst>
 </file>
@@ -497,10 +500,10 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.98"/>
@@ -609,11 +612,21 @@
       <c r="A6" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>44611</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>